<commit_message>
Emoji Sonderzeichen zu FontBitmap hinzugefügt.
</commit_message>
<xml_diff>
--- a/doc/7_Segment_8x5_Konstanten_Rechnerxlsx.xlsx
+++ b/doc/7_Segment_8x5_Konstanten_Rechnerxlsx.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Documents\Projekte\LED-Matrix-WS2812\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AD7A3D-801E-44C1-854D-2D7851494104}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB77E267-363E-4A74-8F37-19D05BF77BE3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="11472" xr2:uid="{1E9B2583-D78D-4AE3-B807-5487FDF5E2B0}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="11472" xr2:uid="{1E9B2583-D78D-4AE3-B807-5487FDF5E2B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>DEZ</t>
   </si>
   <si>
     <t>HEX</t>
+  </si>
+  <si>
+    <t>Heart</t>
+  </si>
+  <si>
+    <t>Smilie</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -172,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -208,6 +223,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -527,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9CFAB04-09CB-45F1-875A-1BC0E081CE5F}">
-  <dimension ref="A1:CB14"/>
+  <dimension ref="A1:CB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D14"/>
+    <sheetView tabSelected="1" topLeftCell="N13" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.109375" defaultRowHeight="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -539,118 +557,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13">
-        <v>1</v>
-      </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13">
+      <c r="A1" s="14">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14">
+        <v>1</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14">
         <v>2</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13">
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14">
         <v>3</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14">
         <v>4</v>
       </c>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13">
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14">
         <v>5</v>
       </c>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13">
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14">
         <v>6</v>
       </c>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13">
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14">
         <v>7</v>
       </c>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13">
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14">
         <v>8</v>
       </c>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13">
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="14"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14">
         <v>9</v>
       </c>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13">
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14">
         <v>10</v>
       </c>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13">
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14">
         <v>11</v>
       </c>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13"/>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13">
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="14"/>
+      <c r="BH1" s="14"/>
+      <c r="BI1" s="14">
         <v>12</v>
       </c>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13"/>
-      <c r="BN1" s="13">
+      <c r="BJ1" s="14"/>
+      <c r="BK1" s="14"/>
+      <c r="BL1" s="14"/>
+      <c r="BM1" s="14"/>
+      <c r="BN1" s="14">
         <v>13</v>
       </c>
-      <c r="BO1" s="13"/>
-      <c r="BP1" s="13"/>
-      <c r="BQ1" s="13"/>
-      <c r="BR1" s="13"/>
-      <c r="BS1" s="13">
+      <c r="BO1" s="14"/>
+      <c r="BP1" s="14"/>
+      <c r="BQ1" s="14"/>
+      <c r="BR1" s="14"/>
+      <c r="BS1" s="14">
         <v>14</v>
       </c>
-      <c r="BT1" s="13"/>
-      <c r="BU1" s="13"/>
-      <c r="BV1" s="13"/>
-      <c r="BW1" s="13"/>
-      <c r="BX1" s="13">
+      <c r="BT1" s="14"/>
+      <c r="BU1" s="14"/>
+      <c r="BV1" s="14"/>
+      <c r="BW1" s="14"/>
+      <c r="BX1" s="14">
         <v>15</v>
       </c>
-      <c r="BY1" s="13"/>
-      <c r="BZ1" s="13"/>
-      <c r="CA1" s="13"/>
-      <c r="CB1" s="13"/>
+      <c r="BY1" s="14"/>
+      <c r="BZ1" s="14"/>
+      <c r="CA1" s="14"/>
+      <c r="CB1" s="14"/>
     </row>
     <row r="2" spans="1:80" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -2278,14 +2296,1764 @@
         <v>00</v>
       </c>
     </row>
+    <row r="18" spans="1:80" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14">
+        <v>1</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="14">
+        <v>6</v>
+      </c>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14">
+        <v>7</v>
+      </c>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
+      <c r="AM18" s="14"/>
+      <c r="AN18" s="14"/>
+      <c r="AO18" s="14">
+        <v>8</v>
+      </c>
+      <c r="AP18" s="14"/>
+      <c r="AQ18" s="14"/>
+      <c r="AR18" s="14"/>
+      <c r="AS18" s="14"/>
+      <c r="AT18" s="14">
+        <v>9</v>
+      </c>
+      <c r="AU18" s="14"/>
+      <c r="AV18" s="14"/>
+      <c r="AW18" s="14"/>
+      <c r="AX18" s="14"/>
+      <c r="AY18" s="14">
+        <v>10</v>
+      </c>
+      <c r="AZ18" s="14"/>
+      <c r="BA18" s="14"/>
+      <c r="BB18" s="14"/>
+      <c r="BC18" s="14"/>
+      <c r="BD18" s="14">
+        <v>11</v>
+      </c>
+      <c r="BE18" s="14"/>
+      <c r="BF18" s="14"/>
+      <c r="BG18" s="14"/>
+      <c r="BH18" s="14"/>
+      <c r="BI18" s="14">
+        <v>12</v>
+      </c>
+      <c r="BJ18" s="14"/>
+      <c r="BK18" s="14"/>
+      <c r="BL18" s="14"/>
+      <c r="BM18" s="14"/>
+      <c r="BN18" s="14">
+        <v>13</v>
+      </c>
+      <c r="BO18" s="14"/>
+      <c r="BP18" s="14"/>
+      <c r="BQ18" s="14"/>
+      <c r="BR18" s="14"/>
+      <c r="BS18" s="14">
+        <v>14</v>
+      </c>
+      <c r="BT18" s="14"/>
+      <c r="BU18" s="14"/>
+      <c r="BV18" s="14"/>
+      <c r="BW18" s="14"/>
+      <c r="BX18" s="14">
+        <v>15</v>
+      </c>
+      <c r="BY18" s="14"/>
+      <c r="BZ18" s="14"/>
+      <c r="CA18" s="14"/>
+      <c r="CB18" s="14"/>
+    </row>
+    <row r="19" spans="1:80" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="4">
+        <v>1</v>
+      </c>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="4"/>
+      <c r="AK19" s="5"/>
+      <c r="AL19" s="5"/>
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="3"/>
+      <c r="AO19" s="4"/>
+      <c r="AP19" s="5"/>
+      <c r="AQ19" s="5"/>
+      <c r="AR19" s="2"/>
+      <c r="AS19" s="3"/>
+      <c r="AT19" s="4"/>
+      <c r="AU19" s="5"/>
+      <c r="AV19" s="5"/>
+      <c r="AW19" s="2"/>
+      <c r="AX19" s="3"/>
+      <c r="AY19" s="4"/>
+      <c r="AZ19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BA19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="3"/>
+      <c r="BD19" s="4"/>
+      <c r="BE19" s="5"/>
+      <c r="BF19" s="5"/>
+      <c r="BG19" s="2"/>
+      <c r="BH19" s="3"/>
+      <c r="BI19" s="4"/>
+      <c r="BJ19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BK19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL19" s="2"/>
+      <c r="BM19" s="3"/>
+      <c r="BN19" s="4"/>
+      <c r="BO19" s="5"/>
+      <c r="BP19" s="5"/>
+      <c r="BQ19" s="2"/>
+      <c r="BR19" s="3"/>
+      <c r="BS19" s="4"/>
+      <c r="BT19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BU19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BV19" s="2"/>
+      <c r="BW19" s="3"/>
+      <c r="BX19" s="4"/>
+      <c r="BY19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BZ19" s="5">
+        <v>1</v>
+      </c>
+      <c r="CA19" s="2"/>
+      <c r="CB19" s="3"/>
+    </row>
+    <row r="20" spans="1:80" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5">
+        <v>1</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5">
+        <v>1</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="6">
+        <v>1</v>
+      </c>
+      <c r="U20" s="4"/>
+      <c r="V20" s="5">
+        <v>1</v>
+      </c>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH20" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="5"/>
+      <c r="AL20" s="5"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="6"/>
+      <c r="AO20" s="4"/>
+      <c r="AP20" s="5"/>
+      <c r="AQ20" s="5"/>
+      <c r="AR20" s="5"/>
+      <c r="AS20" s="6"/>
+      <c r="AT20" s="4"/>
+      <c r="AU20" s="5"/>
+      <c r="AV20" s="5"/>
+      <c r="AW20" s="5"/>
+      <c r="AX20" s="6"/>
+      <c r="AY20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ20" s="5"/>
+      <c r="BA20" s="5"/>
+      <c r="BB20" s="5">
+        <v>1</v>
+      </c>
+      <c r="BC20" s="6"/>
+      <c r="BD20" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE20" s="5"/>
+      <c r="BF20" s="5"/>
+      <c r="BG20" s="5"/>
+      <c r="BH20" s="6"/>
+      <c r="BI20" s="4">
+        <v>1</v>
+      </c>
+      <c r="BJ20" s="5"/>
+      <c r="BK20" s="5"/>
+      <c r="BL20" s="5"/>
+      <c r="BM20" s="6"/>
+      <c r="BN20" s="4"/>
+      <c r="BO20" s="5"/>
+      <c r="BP20" s="5"/>
+      <c r="BQ20" s="5">
+        <v>1</v>
+      </c>
+      <c r="BR20" s="6"/>
+      <c r="BS20" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT20" s="5"/>
+      <c r="BU20" s="5"/>
+      <c r="BV20" s="5"/>
+      <c r="BW20" s="6"/>
+      <c r="BX20" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY20" s="5"/>
+      <c r="BZ20" s="5"/>
+      <c r="CA20" s="5"/>
+      <c r="CB20" s="6"/>
+    </row>
+    <row r="21" spans="1:80" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6">
+        <v>1</v>
+      </c>
+      <c r="K21" s="4">
+        <v>1</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5">
+        <v>1</v>
+      </c>
+      <c r="N21" s="5"/>
+      <c r="O21" s="6">
+        <v>1</v>
+      </c>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5">
+        <v>1</v>
+      </c>
+      <c r="T21" s="6">
+        <v>1</v>
+      </c>
+      <c r="U21" s="4"/>
+      <c r="V21" s="5">
+        <v>1</v>
+      </c>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF21" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="5"/>
+      <c r="AH21" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI21" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="6"/>
+      <c r="AO21" s="4"/>
+      <c r="AP21" s="5"/>
+      <c r="AQ21" s="5"/>
+      <c r="AR21" s="5"/>
+      <c r="AS21" s="6"/>
+      <c r="AT21" s="4"/>
+      <c r="AU21" s="5"/>
+      <c r="AV21" s="5"/>
+      <c r="AW21" s="5"/>
+      <c r="AX21" s="6"/>
+      <c r="AY21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ21" s="5"/>
+      <c r="BA21" s="5"/>
+      <c r="BB21" s="5">
+        <v>1</v>
+      </c>
+      <c r="BC21" s="6"/>
+      <c r="BD21" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE21" s="5"/>
+      <c r="BF21" s="5"/>
+      <c r="BG21" s="5"/>
+      <c r="BH21" s="6"/>
+      <c r="BI21" s="4">
+        <v>1</v>
+      </c>
+      <c r="BJ21" s="5"/>
+      <c r="BK21" s="5"/>
+      <c r="BL21" s="5"/>
+      <c r="BM21" s="6"/>
+      <c r="BN21" s="4"/>
+      <c r="BO21" s="5"/>
+      <c r="BP21" s="5"/>
+      <c r="BQ21" s="5">
+        <v>1</v>
+      </c>
+      <c r="BR21" s="6"/>
+      <c r="BS21" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT21" s="5"/>
+      <c r="BU21" s="5"/>
+      <c r="BV21" s="5"/>
+      <c r="BW21" s="6"/>
+      <c r="BX21" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY21" s="5"/>
+      <c r="BZ21" s="5"/>
+      <c r="CA21" s="5"/>
+      <c r="CB21" s="6"/>
+    </row>
+    <row r="22" spans="1:80" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="6">
+        <v>1</v>
+      </c>
+      <c r="P22" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5">
+        <v>1</v>
+      </c>
+      <c r="S22" s="5">
+        <v>1</v>
+      </c>
+      <c r="T22" s="6"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5">
+        <v>1</v>
+      </c>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="5"/>
+      <c r="AL22" s="5"/>
+      <c r="AM22" s="5"/>
+      <c r="AN22" s="6"/>
+      <c r="AO22" s="4"/>
+      <c r="AP22" s="5"/>
+      <c r="AQ22" s="5"/>
+      <c r="AR22" s="5"/>
+      <c r="AS22" s="6"/>
+      <c r="AT22" s="4"/>
+      <c r="AU22" s="5"/>
+      <c r="AV22" s="5"/>
+      <c r="AW22" s="5"/>
+      <c r="AX22" s="6"/>
+      <c r="AY22" s="4"/>
+      <c r="AZ22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BA22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BB22" s="5"/>
+      <c r="BC22" s="6"/>
+      <c r="BD22" s="4"/>
+      <c r="BE22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BF22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BG22" s="5"/>
+      <c r="BH22" s="6"/>
+      <c r="BI22" s="4"/>
+      <c r="BJ22" s="5"/>
+      <c r="BK22" s="5"/>
+      <c r="BL22" s="5"/>
+      <c r="BM22" s="6"/>
+      <c r="BN22" s="4"/>
+      <c r="BO22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BP22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BQ22" s="5"/>
+      <c r="BR22" s="6"/>
+      <c r="BS22" s="4"/>
+      <c r="BT22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BU22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BV22" s="5"/>
+      <c r="BW22" s="6"/>
+      <c r="BX22" s="4"/>
+      <c r="BY22" s="5">
+        <v>1</v>
+      </c>
+      <c r="BZ22" s="5">
+        <v>1</v>
+      </c>
+      <c r="CA22" s="5"/>
+      <c r="CB22" s="6"/>
+    </row>
+    <row r="23" spans="1:80" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5">
+        <v>1</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5">
+        <v>1</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>1</v>
+      </c>
+      <c r="R23" s="5">
+        <v>1</v>
+      </c>
+      <c r="S23" s="5"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="5">
+        <v>1</v>
+      </c>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="4"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="5"/>
+      <c r="AH23" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ23" s="4"/>
+      <c r="AK23" s="5"/>
+      <c r="AL23" s="5"/>
+      <c r="AM23" s="5"/>
+      <c r="AN23" s="6"/>
+      <c r="AO23" s="4"/>
+      <c r="AP23" s="5"/>
+      <c r="AQ23" s="5"/>
+      <c r="AR23" s="5"/>
+      <c r="AS23" s="6"/>
+      <c r="AT23" s="4"/>
+      <c r="AU23" s="5"/>
+      <c r="AV23" s="5"/>
+      <c r="AW23" s="5"/>
+      <c r="AX23" s="6"/>
+      <c r="AY23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ23" s="5"/>
+      <c r="BA23" s="5"/>
+      <c r="BB23" s="5">
+        <v>1</v>
+      </c>
+      <c r="BC23" s="6"/>
+      <c r="BD23" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE23" s="5"/>
+      <c r="BF23" s="5"/>
+      <c r="BG23" s="5">
+        <v>1</v>
+      </c>
+      <c r="BH23" s="6"/>
+      <c r="BI23" s="4">
+        <v>1</v>
+      </c>
+      <c r="BJ23" s="5"/>
+      <c r="BK23" s="5"/>
+      <c r="BL23" s="5"/>
+      <c r="BM23" s="6"/>
+      <c r="BN23" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO23" s="5"/>
+      <c r="BP23" s="5"/>
+      <c r="BQ23" s="5">
+        <v>1</v>
+      </c>
+      <c r="BR23" s="6"/>
+      <c r="BS23" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT23" s="5"/>
+      <c r="BU23" s="5"/>
+      <c r="BV23" s="5"/>
+      <c r="BW23" s="6"/>
+      <c r="BX23" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY23" s="5"/>
+      <c r="BZ23" s="5"/>
+      <c r="CA23" s="5"/>
+      <c r="CB23" s="6"/>
+    </row>
+    <row r="24" spans="1:80" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
+        <v>1</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5">
+        <v>1</v>
+      </c>
+      <c r="N24" s="5"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="5">
+        <v>1</v>
+      </c>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="5">
+        <v>1</v>
+      </c>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="4"/>
+      <c r="AA24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI24" s="6"/>
+      <c r="AJ24" s="4"/>
+      <c r="AK24" s="5"/>
+      <c r="AL24" s="5"/>
+      <c r="AM24" s="5"/>
+      <c r="AN24" s="6"/>
+      <c r="AO24" s="4"/>
+      <c r="AP24" s="5"/>
+      <c r="AQ24" s="5"/>
+      <c r="AR24" s="5"/>
+      <c r="AS24" s="6"/>
+      <c r="AT24" s="4"/>
+      <c r="AU24" s="5"/>
+      <c r="AV24" s="5"/>
+      <c r="AW24" s="5"/>
+      <c r="AX24" s="6"/>
+      <c r="AY24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ24" s="5"/>
+      <c r="BA24" s="5"/>
+      <c r="BB24" s="5">
+        <v>1</v>
+      </c>
+      <c r="BC24" s="6"/>
+      <c r="BD24" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE24" s="5"/>
+      <c r="BF24" s="5"/>
+      <c r="BG24" s="5">
+        <v>1</v>
+      </c>
+      <c r="BH24" s="6"/>
+      <c r="BI24" s="4">
+        <v>1</v>
+      </c>
+      <c r="BJ24" s="5"/>
+      <c r="BK24" s="5"/>
+      <c r="BL24" s="5"/>
+      <c r="BM24" s="6"/>
+      <c r="BN24" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO24" s="5"/>
+      <c r="BP24" s="5"/>
+      <c r="BQ24" s="5">
+        <v>1</v>
+      </c>
+      <c r="BR24" s="6"/>
+      <c r="BS24" s="4">
+        <v>1</v>
+      </c>
+      <c r="BT24" s="5"/>
+      <c r="BU24" s="5"/>
+      <c r="BV24" s="5"/>
+      <c r="BW24" s="6"/>
+      <c r="BX24" s="4">
+        <v>1</v>
+      </c>
+      <c r="BY24" s="5"/>
+      <c r="BZ24" s="5"/>
+      <c r="CA24" s="5"/>
+      <c r="CB24" s="6"/>
+    </row>
+    <row r="25" spans="1:80" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="6">
+        <v>1</v>
+      </c>
+      <c r="K25" s="4"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="4">
+        <v>1</v>
+      </c>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="4"/>
+      <c r="AA25" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC25" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="4"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="5"/>
+      <c r="AM25" s="5"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="4"/>
+      <c r="AP25" s="5"/>
+      <c r="AQ25" s="5"/>
+      <c r="AR25" s="5"/>
+      <c r="AS25" s="6"/>
+      <c r="AT25" s="4"/>
+      <c r="AU25" s="5"/>
+      <c r="AV25" s="5"/>
+      <c r="AW25" s="5"/>
+      <c r="AX25" s="6"/>
+      <c r="AY25" s="4"/>
+      <c r="AZ25" s="5"/>
+      <c r="BA25" s="5"/>
+      <c r="BB25" s="5"/>
+      <c r="BC25" s="6"/>
+      <c r="BD25" s="4"/>
+      <c r="BE25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BF25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BG25" s="5"/>
+      <c r="BH25" s="6"/>
+      <c r="BI25" s="4"/>
+      <c r="BJ25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BK25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL25" s="5"/>
+      <c r="BM25" s="6"/>
+      <c r="BN25" s="4"/>
+      <c r="BO25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BP25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BQ25" s="5"/>
+      <c r="BR25" s="6"/>
+      <c r="BS25" s="4"/>
+      <c r="BT25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BU25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BV25" s="5"/>
+      <c r="BW25" s="6"/>
+      <c r="BX25" s="4"/>
+      <c r="BY25" s="5"/>
+      <c r="BZ25" s="5"/>
+      <c r="CA25" s="5"/>
+      <c r="CB25" s="6"/>
+    </row>
+    <row r="26" spans="1:80" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="13"/>
+      <c r="AB26" s="13"/>
+      <c r="AC26" s="13"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="7"/>
+      <c r="AF26" s="13"/>
+      <c r="AG26" s="13"/>
+      <c r="AH26" s="13"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="7"/>
+      <c r="AK26" s="13"/>
+      <c r="AL26" s="13"/>
+      <c r="AM26" s="13"/>
+      <c r="AN26" s="9"/>
+      <c r="AO26" s="7"/>
+      <c r="AP26" s="13"/>
+      <c r="AQ26" s="13"/>
+      <c r="AR26" s="13"/>
+      <c r="AS26" s="9"/>
+      <c r="AT26" s="7"/>
+      <c r="AU26" s="13"/>
+      <c r="AV26" s="13"/>
+      <c r="AW26" s="13"/>
+      <c r="AX26" s="9"/>
+      <c r="AY26" s="7"/>
+      <c r="AZ26" s="13"/>
+      <c r="BA26" s="13"/>
+      <c r="BB26" s="13"/>
+      <c r="BC26" s="9"/>
+      <c r="BD26" s="7"/>
+      <c r="BE26" s="13"/>
+      <c r="BF26" s="13"/>
+      <c r="BG26" s="13"/>
+      <c r="BH26" s="9"/>
+      <c r="BI26" s="7"/>
+      <c r="BJ26" s="13"/>
+      <c r="BK26" s="13"/>
+      <c r="BL26" s="13"/>
+      <c r="BM26" s="9"/>
+      <c r="BN26" s="7"/>
+      <c r="BO26" s="13"/>
+      <c r="BP26" s="13"/>
+      <c r="BQ26" s="13"/>
+      <c r="BR26" s="9"/>
+      <c r="BS26" s="7"/>
+      <c r="BT26" s="13"/>
+      <c r="BU26" s="13"/>
+      <c r="BV26" s="13"/>
+      <c r="BW26" s="9"/>
+      <c r="BX26" s="7"/>
+      <c r="BY26" s="13"/>
+      <c r="BZ26" s="13"/>
+      <c r="CA26" s="13"/>
+      <c r="CB26" s="9"/>
+    </row>
+    <row r="27" spans="1:80" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:80" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="10">
+        <f>A19*2^0+A20*2^1+A21*2^2+A22*2^3+A23*2^4+A24*2^5+A25*2^6+A26*2^7</f>
+        <v>38</v>
+      </c>
+      <c r="B28" s="11">
+        <f>B19*2^0+B20*2^1+B21*2^2+B22*2^3+B23*2^4+B24*2^5+B25*2^6+B26*2^7</f>
+        <v>70</v>
+      </c>
+      <c r="C28" s="11">
+        <f>C19*2^0+C20*2^1+C21*2^2+C22*2^3+C23*2^4+C24*2^5+C25*2^6+C26*2^7</f>
+        <v>88</v>
+      </c>
+      <c r="D28" s="11">
+        <f>D19*2^0+D20*2^1+D21*2^2+D22*2^3+D23*2^4+D24*2^5+D25*2^6+D26*2^7</f>
+        <v>70</v>
+      </c>
+      <c r="E28" s="12">
+        <f>E19*2^0+E20*2^1+E21*2^2+E22*2^3+E23*2^4+E24*2^5+E25*2^6+E26*2^7</f>
+        <v>38</v>
+      </c>
+      <c r="F28" s="10">
+        <f>F19*2^0+F20*2^1+F21*2^2+F22*2^3+F23*2^4+F24*2^5+F25*2^6+F26*2^7</f>
+        <v>70</v>
+      </c>
+      <c r="G28" s="11">
+        <f>G19*2^0+G20*2^1+G21*2^2+G22*2^3+G23*2^4+G24*2^5+G25*2^6+G26*2^7</f>
+        <v>38</v>
+      </c>
+      <c r="H28" s="11">
+        <f>H19*2^0+H20*2^1+H21*2^2+H22*2^3+H23*2^4+H24*2^5+H25*2^6+H26*2^7</f>
+        <v>56</v>
+      </c>
+      <c r="I28" s="11">
+        <f>I19*2^0+I20*2^1+I21*2^2+I22*2^3+I23*2^4+I24*2^5+I25*2^6+I26*2^7</f>
+        <v>38</v>
+      </c>
+      <c r="J28" s="12">
+        <f t="shared" ref="J28:BU28" si="5">J19*2^0+J20*2^1+J21*2^2+J22*2^3+J23*2^4+J24*2^5+J25*2^6+J26*2^7</f>
+        <v>70</v>
+      </c>
+      <c r="K28" s="10">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="L28" s="11">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="M28" s="11">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="N28" s="11">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="O28" s="12">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="P28" s="10">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="Q28" s="11">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="R28" s="11">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="S28" s="11">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="T28" s="12">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="U28" s="10">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="V28" s="11">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="W28" s="11">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="X28" s="11">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="Y28" s="12">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="Z28" s="10">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="AA28" s="11">
+        <f t="shared" si="5"/>
+        <v>103</v>
+      </c>
+      <c r="AB28" s="11">
+        <f t="shared" si="5"/>
+        <v>111</v>
+      </c>
+      <c r="AC28" s="11">
+        <f t="shared" si="5"/>
+        <v>103</v>
+      </c>
+      <c r="AD28" s="12">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="AE28" s="10">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AF28" s="11">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="AG28" s="11">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="AH28" s="11">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="AI28" s="12">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AJ28" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AK28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AL28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AM28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AN28" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AO28" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AP28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AQ28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AR28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AS28" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AT28" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AU28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AV28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AW28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AX28" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AY28" s="10">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="AZ28" s="11">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="BA28" s="11">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="BB28" s="11">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="BC28" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BD28" s="10">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="BE28" s="11">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="BF28" s="11">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="BG28" s="11">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="BH28" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BI28" s="10">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="BJ28" s="11">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="BK28" s="11">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="BL28" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BM28" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BN28" s="10">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="BO28" s="11">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="BP28" s="11">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="BQ28" s="11">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="BR28" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BS28" s="10">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+      <c r="BT28" s="11">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="BU28" s="11">
+        <f t="shared" si="5"/>
+        <v>73</v>
+      </c>
+      <c r="BV28" s="11">
+        <f t="shared" ref="BV28:CB28" si="6">BV19*2^0+BV20*2^1+BV21*2^2+BV22*2^3+BV23*2^4+BV24*2^5+BV25*2^6+BV26*2^7</f>
+        <v>0</v>
+      </c>
+      <c r="BW28" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="BX28" s="10">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
+      <c r="BY28" s="11">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="BZ28" s="11">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="CA28" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="CB28" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:80" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:80" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="str">
+        <f>DEC2HEX(A28,2)</f>
+        <v>26</v>
+      </c>
+      <c r="B31" s="11" t="str">
+        <f t="shared" ref="B31:D31" si="7">DEC2HEX(B28,2)</f>
+        <v>46</v>
+      </c>
+      <c r="C31" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>58</v>
+      </c>
+      <c r="D31" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>46</v>
+      </c>
+      <c r="E31" s="12" t="str">
+        <f>DEC2HEX(E28,2)</f>
+        <v>26</v>
+      </c>
+      <c r="F31" s="10" t="str">
+        <f t="shared" ref="F31:BQ31" si="8">DEC2HEX(F28,2)</f>
+        <v>46</v>
+      </c>
+      <c r="G31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="H31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>38</v>
+      </c>
+      <c r="I31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="J31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>46</v>
+      </c>
+      <c r="K31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>0C</v>
+      </c>
+      <c r="L31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="M31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="N31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="O31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>0C</v>
+      </c>
+      <c r="P31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="Q31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="R31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="S31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>0C</v>
+      </c>
+      <c r="T31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>06</v>
+      </c>
+      <c r="U31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>41</v>
+      </c>
+      <c r="V31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="W31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>08</v>
+      </c>
+      <c r="X31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="Y31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>41</v>
+      </c>
+      <c r="Z31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>03</v>
+      </c>
+      <c r="AA31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>67</v>
+      </c>
+      <c r="AB31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>6F</v>
+      </c>
+      <c r="AC31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>67</v>
+      </c>
+      <c r="AD31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>03</v>
+      </c>
+      <c r="AE31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>1C</v>
+      </c>
+      <c r="AF31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="AG31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>2A</v>
+      </c>
+      <c r="AH31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="AI31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>1C</v>
+      </c>
+      <c r="AJ31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AK31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AL31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AM31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AN31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AO31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AP31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AQ31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AR31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AS31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AT31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AU31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AV31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AW31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AX31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="AY31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="AZ31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>09</v>
+      </c>
+      <c r="BA31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>09</v>
+      </c>
+      <c r="BB31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="BC31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="BD31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="BE31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
+      <c r="BF31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
+      <c r="BG31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="BH31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="BI31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="BJ31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>41</v>
+      </c>
+      <c r="BK31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>41</v>
+      </c>
+      <c r="BL31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="BM31" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>00</v>
+      </c>
+      <c r="BN31" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="BO31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
+      <c r="BP31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
+      <c r="BQ31" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="BR31" s="12" t="str">
+        <f t="shared" ref="BR31:CB31" si="9">DEC2HEX(BR28,2)</f>
+        <v>00</v>
+      </c>
+      <c r="BS31" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="BT31" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>49</v>
+      </c>
+      <c r="BU31" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>49</v>
+      </c>
+      <c r="BV31" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>00</v>
+      </c>
+      <c r="BW31" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v>00</v>
+      </c>
+      <c r="BX31" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+      <c r="BY31" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>09</v>
+      </c>
+      <c r="BZ31" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>09</v>
+      </c>
+      <c r="CA31" s="11" t="str">
+        <f t="shared" si="9"/>
+        <v>00</v>
+      </c>
+      <c r="CB31" s="12" t="str">
+        <f t="shared" si="9"/>
+        <v>00</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="U1:Y1"/>
+  <mergeCells count="32">
+    <mergeCell ref="BX18:CB18"/>
+    <mergeCell ref="AY18:BC18"/>
+    <mergeCell ref="BD18:BH18"/>
+    <mergeCell ref="BI18:BM18"/>
+    <mergeCell ref="BN18:BR18"/>
+    <mergeCell ref="BS18:BW18"/>
+    <mergeCell ref="Z18:AD18"/>
+    <mergeCell ref="AE18:AI18"/>
+    <mergeCell ref="AJ18:AN18"/>
+    <mergeCell ref="AO18:AS18"/>
+    <mergeCell ref="AT18:AX18"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="K18:O18"/>
+    <mergeCell ref="P18:T18"/>
+    <mergeCell ref="U18:Y18"/>
     <mergeCell ref="BI1:BM1"/>
     <mergeCell ref="BN1:BR1"/>
     <mergeCell ref="BS1:BW1"/>
@@ -2296,6 +4064,12 @@
     <mergeCell ref="AT1:AX1"/>
     <mergeCell ref="AY1:BC1"/>
     <mergeCell ref="BD1:BH1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>